<commit_message>
Ajustes da tabela em excel, com as nomenclaturas e mudanças de acordo com a implementação no SQL
</commit_message>
<xml_diff>
--- a/SpotifyClone-NormalizedTable.xlsx
+++ b/SpotifyClone-NormalizedTable.xlsx
@@ -9,7 +9,7 @@
     <sheet state="visible" name="songs" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="albums" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="users" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="following artists" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="following_artists" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>artist_id</t>
   </si>
@@ -46,27 +46,24 @@
     <t>plan_id</t>
   </si>
   <si>
-    <t>value</t>
+    <t>price</t>
   </si>
   <si>
     <t>gratuito</t>
   </si>
   <si>
+    <t>universitário</t>
+  </si>
+  <si>
+    <t>5.99</t>
+  </si>
+  <si>
     <t>familiar</t>
   </si>
   <si>
     <t>7.99</t>
   </si>
   <si>
-    <t>universitário</t>
-  </si>
-  <si>
-    <t>5.99</t>
-  </si>
-  <si>
-    <t>song_name</t>
-  </si>
-  <si>
     <t>album_id</t>
   </si>
   <si>
@@ -97,7 +94,7 @@
     <t>She Knows</t>
   </si>
   <si>
-    <t>Fantasy For Me"</t>
+    <t>Fantasy For Me</t>
   </si>
   <si>
     <t>Celebration Of More</t>
@@ -152,9 +149,6 @@
   </si>
   <si>
     <t>Roger</t>
-  </si>
-  <si>
-    <t>usuario_id</t>
   </si>
   <si>
     <t>artista_id</t>
@@ -712,7 +706,7 @@
       <c r="A3" s="1">
         <v>2.0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -723,12 +717,16 @@
       <c r="A4" s="1">
         <v>3.0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -753,10 +751,10 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2">
@@ -764,7 +762,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1">
         <v>1.0</v>
@@ -775,7 +773,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1">
         <v>1.0</v>
@@ -786,7 +784,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1">
         <v>1.0</v>
@@ -797,7 +795,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1">
         <v>2.0</v>
@@ -808,7 +806,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
@@ -819,7 +817,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
         <v>3.0</v>
@@ -830,7 +828,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1">
         <v>3.0</v>
@@ -841,7 +839,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1">
         <v>3.0</v>
@@ -852,7 +850,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1">
         <v>3.0</v>
@@ -863,7 +861,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
         <v>4.0</v>
@@ -874,7 +872,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1">
         <v>4.0</v>
@@ -885,7 +883,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1">
         <v>4.0</v>
@@ -896,7 +894,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1">
         <v>4.0</v>
@@ -907,7 +905,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1">
         <v>4.0</v>
@@ -918,7 +916,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1">
         <v>4.0</v>
@@ -929,7 +927,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1">
         <v>5.0</v>
@@ -940,7 +938,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1">
         <v>5.0</v>
@@ -951,7 +949,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1">
         <v>5.0</v>
@@ -977,7 +975,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -991,7 +989,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1">
         <v>1.0</v>
@@ -1002,7 +1000,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1">
         <v>1.0</v>
@@ -1013,7 +1011,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1">
         <v>2.0</v>
@@ -1024,7 +1022,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1">
         <v>3.0</v>
@@ -1035,7 +1033,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1">
         <v>4.0</v>
@@ -1064,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1075,7 +1073,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1">
         <v>23.0</v>
@@ -1089,13 +1087,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1">
         <v>35.0</v>
       </c>
       <c r="D3" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
@@ -1103,13 +1101,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1">
         <v>20.0</v>
       </c>
       <c r="D4" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
@@ -1117,7 +1115,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1">
         <v>45.0</v>
@@ -1143,10 +1141,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2">

</xml_diff>